<commit_message>
Unified column names for all datasets
</commit_message>
<xml_diff>
--- a/Cleaned-Data/2018-Passouts/Sem-3_2018_Passout_cleaned.xlsx
+++ b/Cleaned-Data/2018-Passouts/Sem-3_2018_Passout_cleaned.xlsx
@@ -101,9 +101,6 @@
     <t>P/F</t>
   </si>
   <si>
-    <t>CGPA</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -729,6 +726,9 @@
   </si>
   <si>
     <t>TAMBE SONALI SUNIL</t>
+  </si>
+  <si>
+    <t>GPA</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
@@ -1139,13 +1139,13 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>0</v>
@@ -1211,12 +1211,12 @@
         <v>22</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>23</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="5">
         <v>0</v>
@@ -1293,7 +1293,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="5">
         <v>0</v>
@@ -1370,7 +1370,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="5">
         <v>0</v>
@@ -1447,7 +1447,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B5" s="5">
         <v>1</v>
@@ -1524,7 +1524,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="5">
         <v>0</v>
@@ -1601,7 +1601,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B7" s="5">
         <v>1</v>
@@ -1678,7 +1678,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
@@ -1755,7 +1755,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="5">
         <v>0</v>
@@ -1832,7 +1832,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="5">
         <v>0</v>
@@ -1909,7 +1909,7 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B11" s="5">
         <v>1</v>
@@ -1986,7 +1986,7 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="5">
         <v>0</v>
@@ -2063,7 +2063,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B13" s="5">
         <v>1</v>
@@ -2140,7 +2140,7 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="5">
         <v>0</v>
@@ -2217,7 +2217,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="5">
         <v>0</v>
@@ -2294,7 +2294,7 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B16" s="5">
         <v>1</v>
@@ -2371,7 +2371,7 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="5">
         <v>0</v>
@@ -2448,7 +2448,7 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18" s="5">
         <v>0</v>
@@ -2525,7 +2525,7 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="5">
         <v>0</v>
@@ -2602,7 +2602,7 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B20" s="5">
         <v>1</v>
@@ -2679,7 +2679,7 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" s="5">
         <v>0</v>
@@ -2756,7 +2756,7 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B22" s="5">
         <v>1</v>
@@ -2833,7 +2833,7 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B23" s="5">
         <v>1</v>
@@ -2910,7 +2910,7 @@
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B24" s="5">
         <v>1</v>
@@ -2987,7 +2987,7 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="5">
         <v>0</v>
@@ -3064,7 +3064,7 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B26" s="5">
         <v>1</v>
@@ -3141,7 +3141,7 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" s="5">
         <v>0</v>
@@ -3218,7 +3218,7 @@
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" s="5">
         <v>0</v>
@@ -3295,7 +3295,7 @@
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29" s="5">
         <v>0</v>
@@ -3372,7 +3372,7 @@
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30" s="5">
         <v>0</v>
@@ -3449,7 +3449,7 @@
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B31" s="5">
         <v>1</v>
@@ -3526,7 +3526,7 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B32" s="5">
         <v>0</v>
@@ -3603,7 +3603,7 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B33" s="5">
         <v>1</v>
@@ -3680,7 +3680,7 @@
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B34" s="5">
         <v>0</v>
@@ -3757,7 +3757,7 @@
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B35" s="5">
         <v>0</v>
@@ -3834,7 +3834,7 @@
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B36" s="5">
         <v>0</v>
@@ -3911,7 +3911,7 @@
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B37" s="5">
         <v>0</v>
@@ -3988,7 +3988,7 @@
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B38" s="5">
         <v>1</v>
@@ -4065,7 +4065,7 @@
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B39" s="5">
         <v>1</v>
@@ -4142,7 +4142,7 @@
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B40" s="5">
         <v>0</v>
@@ -4219,7 +4219,7 @@
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B41" s="5">
         <v>0</v>
@@ -4296,7 +4296,7 @@
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B42" s="5">
         <v>0</v>
@@ -4373,7 +4373,7 @@
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B43" s="5">
         <v>0</v>
@@ -4450,7 +4450,7 @@
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B44" s="5">
         <v>0</v>
@@ -4527,7 +4527,7 @@
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B45" s="5">
         <v>0</v>
@@ -4604,7 +4604,7 @@
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B46" s="5">
         <v>0</v>
@@ -4681,7 +4681,7 @@
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B47" s="5">
         <v>0</v>
@@ -4758,7 +4758,7 @@
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B48" s="5">
         <v>0</v>
@@ -4835,7 +4835,7 @@
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B49" s="5">
         <v>0</v>
@@ -4912,7 +4912,7 @@
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B50" s="5">
         <v>0</v>
@@ -4989,7 +4989,7 @@
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B51" s="5">
         <v>1</v>
@@ -5066,7 +5066,7 @@
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B52" s="5">
         <v>1</v>
@@ -5143,7 +5143,7 @@
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B53" s="5">
         <v>0</v>
@@ -5220,7 +5220,7 @@
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B54" s="5">
         <v>1</v>
@@ -5297,7 +5297,7 @@
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B55" s="5">
         <v>0</v>
@@ -5374,7 +5374,7 @@
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B56" s="5">
         <v>0</v>
@@ -5451,7 +5451,7 @@
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B57" s="5">
         <v>0</v>
@@ -5528,7 +5528,7 @@
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B58" s="5">
         <v>1</v>
@@ -5605,7 +5605,7 @@
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B59" s="5">
         <v>0</v>
@@ -5682,7 +5682,7 @@
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B60" s="5">
         <v>0</v>
@@ -5759,7 +5759,7 @@
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B61" s="5">
         <v>0</v>
@@ -5836,7 +5836,7 @@
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B62" s="5">
         <v>1</v>
@@ -5913,7 +5913,7 @@
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B63" s="5">
         <v>0</v>
@@ -5990,7 +5990,7 @@
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B64" s="5">
         <v>1</v>
@@ -6067,7 +6067,7 @@
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B65" s="5">
         <v>1</v>
@@ -6144,7 +6144,7 @@
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B66" s="5">
         <v>0</v>
@@ -6221,7 +6221,7 @@
     </row>
     <row r="67" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B67" s="5">
         <v>0</v>
@@ -6298,7 +6298,7 @@
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B68" s="5">
         <v>0</v>
@@ -6375,7 +6375,7 @@
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B69" s="5">
         <v>0</v>
@@ -6452,7 +6452,7 @@
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B70" s="5">
         <v>0</v>
@@ -6529,7 +6529,7 @@
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B71" s="5">
         <v>0</v>
@@ -6606,7 +6606,7 @@
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B72" s="5">
         <v>0</v>
@@ -6683,7 +6683,7 @@
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B73" s="5">
         <v>0</v>
@@ -6760,7 +6760,7 @@
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B74" s="5">
         <v>0</v>
@@ -6837,7 +6837,7 @@
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B75" s="5">
         <v>1</v>
@@ -6914,7 +6914,7 @@
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B76" s="5">
         <v>0</v>
@@ -6991,7 +6991,7 @@
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B77" s="5">
         <v>0</v>
@@ -7068,7 +7068,7 @@
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B78" s="5">
         <v>1</v>
@@ -7145,7 +7145,7 @@
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B79" s="5">
         <v>0</v>
@@ -7222,7 +7222,7 @@
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B80" s="5">
         <v>0</v>
@@ -7299,7 +7299,7 @@
     </row>
     <row r="81" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B81" s="5">
         <v>1</v>
@@ -7376,7 +7376,7 @@
     </row>
     <row r="82" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B82" s="5">
         <v>0</v>
@@ -7453,7 +7453,7 @@
     </row>
     <row r="83" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B83" s="5">
         <v>1</v>
@@ -7530,7 +7530,7 @@
     </row>
     <row r="84" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B84" s="5">
         <v>0</v>
@@ -7607,7 +7607,7 @@
     </row>
     <row r="85" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B85" s="5">
         <v>1</v>
@@ -7684,7 +7684,7 @@
     </row>
     <row r="86" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B86" s="5">
         <v>0</v>
@@ -7761,7 +7761,7 @@
     </row>
     <row r="87" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B87" s="5">
         <v>1</v>
@@ -7838,7 +7838,7 @@
     </row>
     <row r="88" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A88" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B88" s="5">
         <v>0</v>
@@ -7915,7 +7915,7 @@
     </row>
     <row r="89" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B89" s="5">
         <v>1</v>
@@ -7992,7 +7992,7 @@
     </row>
     <row r="90" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A90" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B90" s="5">
         <v>0</v>
@@ -8069,7 +8069,7 @@
     </row>
     <row r="91" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A91" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B91" s="5">
         <v>1</v>
@@ -8146,7 +8146,7 @@
     </row>
     <row r="92" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B92" s="5">
         <v>0</v>
@@ -8223,7 +8223,7 @@
     </row>
     <row r="93" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B93" s="5">
         <v>0</v>
@@ -8300,7 +8300,7 @@
     </row>
     <row r="94" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B94" s="5">
         <v>1</v>
@@ -8377,7 +8377,7 @@
     </row>
     <row r="95" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B95" s="5">
         <v>0</v>
@@ -8454,7 +8454,7 @@
     </row>
     <row r="96" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B96" s="5">
         <v>0</v>
@@ -8531,7 +8531,7 @@
     </row>
     <row r="97" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B97" s="5">
         <v>0</v>
@@ -8608,7 +8608,7 @@
     </row>
     <row r="98" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A98" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B98" s="5">
         <v>0</v>
@@ -8685,7 +8685,7 @@
     </row>
     <row r="99" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B99" s="5">
         <v>0</v>
@@ -8762,7 +8762,7 @@
     </row>
     <row r="100" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A100" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B100" s="5">
         <v>0</v>
@@ -8839,7 +8839,7 @@
     </row>
     <row r="101" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B101" s="5">
         <v>0</v>
@@ -8916,7 +8916,7 @@
     </row>
     <row r="102" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B102" s="5">
         <v>0</v>
@@ -8993,7 +8993,7 @@
     </row>
     <row r="103" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A103" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B103" s="5">
         <v>0</v>
@@ -9070,7 +9070,7 @@
     </row>
     <row r="104" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A104" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B104" s="5">
         <v>0</v>
@@ -9147,7 +9147,7 @@
     </row>
     <row r="105" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A105" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B105" s="5">
         <v>1</v>
@@ -9224,7 +9224,7 @@
     </row>
     <row r="106" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A106" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B106" s="5">
         <v>1</v>
@@ -9301,7 +9301,7 @@
     </row>
     <row r="107" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B107" s="5">
         <v>0</v>
@@ -9378,7 +9378,7 @@
     </row>
     <row r="108" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B108" s="5">
         <v>0</v>
@@ -9455,7 +9455,7 @@
     </row>
     <row r="109" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B109" s="5">
         <v>0</v>
@@ -9532,7 +9532,7 @@
     </row>
     <row r="110" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A110" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B110" s="5">
         <v>0</v>
@@ -9609,7 +9609,7 @@
     </row>
     <row r="111" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B111" s="5">
         <v>1</v>
@@ -9686,7 +9686,7 @@
     </row>
     <row r="112" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B112" s="5">
         <v>0</v>
@@ -9763,7 +9763,7 @@
     </row>
     <row r="113" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B113" s="5">
         <v>0</v>
@@ -9840,7 +9840,7 @@
     </row>
     <row r="114" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A114" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B114" s="5">
         <v>0</v>
@@ -9917,7 +9917,7 @@
     </row>
     <row r="115" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B115" s="5">
         <v>0</v>
@@ -9994,7 +9994,7 @@
     </row>
     <row r="116" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A116" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B116" s="5">
         <v>1</v>
@@ -10071,7 +10071,7 @@
     </row>
     <row r="117" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A117" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B117" s="5">
         <v>0</v>
@@ -10148,7 +10148,7 @@
     </row>
     <row r="118" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A118" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B118" s="5">
         <v>0</v>
@@ -10225,7 +10225,7 @@
     </row>
     <row r="119" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A119" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B119" s="5">
         <v>0</v>
@@ -10302,7 +10302,7 @@
     </row>
     <row r="120" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A120" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B120" s="5">
         <v>0</v>
@@ -10379,7 +10379,7 @@
     </row>
     <row r="121" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A121" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B121" s="5">
         <v>0</v>
@@ -10456,7 +10456,7 @@
     </row>
     <row r="122" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A122" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B122" s="5">
         <v>1</v>
@@ -10533,7 +10533,7 @@
     </row>
     <row r="123" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A123" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B123" s="5">
         <v>0</v>
@@ -10610,7 +10610,7 @@
     </row>
     <row r="124" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A124" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B124" s="5">
         <v>0</v>
@@ -10687,7 +10687,7 @@
     </row>
     <row r="125" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A125" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B125" s="5">
         <v>1</v>
@@ -10764,7 +10764,7 @@
     </row>
     <row r="126" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A126" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B126" s="5">
         <v>0</v>
@@ -10841,7 +10841,7 @@
     </row>
     <row r="127" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A127" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B127" s="5">
         <v>1</v>
@@ -10918,7 +10918,7 @@
     </row>
     <row r="128" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A128" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B128" s="5">
         <v>0</v>
@@ -10995,7 +10995,7 @@
     </row>
     <row r="129" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A129" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B129" s="5">
         <v>0</v>
@@ -11072,7 +11072,7 @@
     </row>
     <row r="130" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A130" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B130" s="5">
         <v>0</v>
@@ -11149,7 +11149,7 @@
     </row>
     <row r="131" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A131" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B131" s="5">
         <v>0</v>
@@ -11226,7 +11226,7 @@
     </row>
     <row r="132" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A132" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B132" s="5">
         <v>0</v>
@@ -11303,7 +11303,7 @@
     </row>
     <row r="133" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A133" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B133" s="5">
         <v>0</v>
@@ -11380,7 +11380,7 @@
     </row>
     <row r="134" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A134" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B134" s="5">
         <v>0</v>
@@ -11457,7 +11457,7 @@
     </row>
     <row r="135" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A135" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B135" s="5">
         <v>0</v>
@@ -11534,7 +11534,7 @@
     </row>
     <row r="136" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A136" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B136" s="5">
         <v>0</v>
@@ -11611,7 +11611,7 @@
     </row>
     <row r="137" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A137" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B137" s="5">
         <v>1</v>
@@ -11688,7 +11688,7 @@
     </row>
     <row r="138" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A138" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B138" s="5">
         <v>0</v>
@@ -11765,7 +11765,7 @@
     </row>
     <row r="139" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A139" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B139" s="5">
         <v>1</v>
@@ -11842,7 +11842,7 @@
     </row>
     <row r="140" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A140" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B140" s="5">
         <v>0</v>
@@ -11919,7 +11919,7 @@
     </row>
     <row r="141" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A141" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B141" s="5">
         <v>1</v>
@@ -11996,7 +11996,7 @@
     </row>
     <row r="142" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A142" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B142" s="5">
         <v>0</v>
@@ -12073,7 +12073,7 @@
     </row>
     <row r="143" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A143" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B143" s="5">
         <v>0</v>
@@ -12150,7 +12150,7 @@
     </row>
     <row r="144" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A144" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B144" s="5">
         <v>0</v>
@@ -12227,7 +12227,7 @@
     </row>
     <row r="145" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A145" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B145" s="5">
         <v>0</v>
@@ -12304,7 +12304,7 @@
     </row>
     <row r="146" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A146" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B146" s="5">
         <v>0</v>
@@ -12381,7 +12381,7 @@
     </row>
     <row r="147" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A147" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B147" s="5">
         <v>0</v>
@@ -12458,7 +12458,7 @@
     </row>
     <row r="148" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A148" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B148" s="5">
         <v>1</v>
@@ -12535,7 +12535,7 @@
     </row>
     <row r="149" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A149" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B149" s="5">
         <v>1</v>
@@ -12612,7 +12612,7 @@
     </row>
     <row r="150" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A150" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B150" s="5">
         <v>0</v>
@@ -12689,7 +12689,7 @@
     </row>
     <row r="151" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A151" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B151" s="5">
         <v>1</v>
@@ -12766,7 +12766,7 @@
     </row>
     <row r="152" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A152" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B152" s="5">
         <v>1</v>
@@ -12843,7 +12843,7 @@
     </row>
     <row r="153" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A153" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B153" s="5">
         <v>0</v>
@@ -12920,7 +12920,7 @@
     </row>
     <row r="154" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A154" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B154" s="5">
         <v>0</v>
@@ -12997,7 +12997,7 @@
     </row>
     <row r="155" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A155" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B155" s="5">
         <v>0</v>
@@ -13074,7 +13074,7 @@
     </row>
     <row r="156" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A156" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B156" s="5">
         <v>0</v>
@@ -13151,7 +13151,7 @@
     </row>
     <row r="157" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A157" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B157" s="5">
         <v>0</v>
@@ -13228,7 +13228,7 @@
     </row>
     <row r="158" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A158" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B158" s="5">
         <v>0</v>
@@ -13305,7 +13305,7 @@
     </row>
     <row r="159" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A159" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B159" s="5">
         <v>0</v>
@@ -13382,7 +13382,7 @@
     </row>
     <row r="160" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A160" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B160" s="5">
         <v>0</v>
@@ -13459,7 +13459,7 @@
     </row>
     <row r="161" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A161" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B161" s="5">
         <v>0</v>
@@ -13536,7 +13536,7 @@
     </row>
     <row r="162" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A162" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B162" s="5">
         <v>0</v>
@@ -13613,7 +13613,7 @@
     </row>
     <row r="163" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A163" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B163" s="5">
         <v>0</v>
@@ -13690,7 +13690,7 @@
     </row>
     <row r="164" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A164" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B164" s="5">
         <v>0</v>
@@ -13767,7 +13767,7 @@
     </row>
     <row r="165" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A165" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B165" s="5">
         <v>0</v>
@@ -13844,7 +13844,7 @@
     </row>
     <row r="166" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A166" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B166" s="5">
         <v>0</v>
@@ -13921,7 +13921,7 @@
     </row>
     <row r="167" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A167" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B167" s="5">
         <v>0</v>
@@ -13998,7 +13998,7 @@
     </row>
     <row r="168" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A168" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B168" s="5">
         <v>0</v>
@@ -14075,7 +14075,7 @@
     </row>
     <row r="169" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A169" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B169" s="5">
         <v>0</v>
@@ -14152,7 +14152,7 @@
     </row>
     <row r="170" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A170" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B170" s="5">
         <v>0</v>
@@ -14229,7 +14229,7 @@
     </row>
     <row r="171" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A171" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B171" s="5">
         <v>0</v>
@@ -14306,7 +14306,7 @@
     </row>
     <row r="172" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A172" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B172" s="5">
         <v>0</v>
@@ -14383,7 +14383,7 @@
     </row>
     <row r="173" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A173" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B173" s="5">
         <v>0</v>
@@ -14460,7 +14460,7 @@
     </row>
     <row r="174" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A174" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B174" s="5">
         <v>1</v>
@@ -14537,7 +14537,7 @@
     </row>
     <row r="175" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A175" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B175" s="5">
         <v>0</v>
@@ -14614,7 +14614,7 @@
     </row>
     <row r="176" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A176" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B176" s="5">
         <v>1</v>
@@ -14691,7 +14691,7 @@
     </row>
     <row r="177" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A177" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B177" s="5">
         <v>0</v>
@@ -14768,7 +14768,7 @@
     </row>
     <row r="178" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A178" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B178" s="5">
         <v>0</v>
@@ -14845,7 +14845,7 @@
     </row>
     <row r="179" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A179" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B179" s="5">
         <v>0</v>
@@ -14922,7 +14922,7 @@
     </row>
     <row r="180" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A180" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B180" s="5">
         <v>0</v>
@@ -14999,7 +14999,7 @@
     </row>
     <row r="181" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A181" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B181" s="5">
         <v>0</v>
@@ -15076,7 +15076,7 @@
     </row>
     <row r="182" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A182" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B182" s="5">
         <v>0</v>
@@ -15153,7 +15153,7 @@
     </row>
     <row r="183" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A183" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B183" s="5">
         <v>0</v>
@@ -15230,7 +15230,7 @@
     </row>
     <row r="184" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A184" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B184" s="5">
         <v>0</v>
@@ -15307,7 +15307,7 @@
     </row>
     <row r="185" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A185" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B185" s="5">
         <v>1</v>
@@ -15384,7 +15384,7 @@
     </row>
     <row r="186" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A186" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B186" s="5">
         <v>0</v>
@@ -15461,7 +15461,7 @@
     </row>
     <row r="187" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A187" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B187" s="5">
         <v>0</v>
@@ -15538,7 +15538,7 @@
     </row>
     <row r="188" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A188" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B188" s="5">
         <v>1</v>
@@ -15615,7 +15615,7 @@
     </row>
     <row r="189" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A189" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B189" s="5">
         <v>1</v>
@@ -15692,7 +15692,7 @@
     </row>
     <row r="190" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A190" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B190" s="5">
         <v>0</v>
@@ -15769,7 +15769,7 @@
     </row>
     <row r="191" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A191" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B191" s="5">
         <v>1</v>
@@ -15846,7 +15846,7 @@
     </row>
     <row r="192" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A192" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B192" s="5">
         <v>0</v>
@@ -15923,7 +15923,7 @@
     </row>
     <row r="193" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A193" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B193" s="5">
         <v>0</v>
@@ -16000,7 +16000,7 @@
     </row>
     <row r="194" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A194" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B194" s="5">
         <v>0</v>
@@ -16077,7 +16077,7 @@
     </row>
     <row r="195" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A195" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B195" s="5">
         <v>0</v>
@@ -16154,7 +16154,7 @@
     </row>
     <row r="196" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A196" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B196" s="5">
         <v>0</v>
@@ -16231,7 +16231,7 @@
     </row>
     <row r="197" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A197" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B197" s="5">
         <v>0</v>
@@ -16308,7 +16308,7 @@
     </row>
     <row r="198" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A198" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B198" s="5">
         <v>0</v>
@@ -16385,7 +16385,7 @@
     </row>
     <row r="199" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A199" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B199" s="5">
         <v>0</v>
@@ -16462,7 +16462,7 @@
     </row>
     <row r="200" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A200" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B200" s="5">
         <v>0</v>
@@ -16539,7 +16539,7 @@
     </row>
     <row r="201" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A201" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B201" s="5">
         <v>0</v>
@@ -16616,7 +16616,7 @@
     </row>
     <row r="202" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A202" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B202" s="5">
         <v>0</v>
@@ -16693,7 +16693,7 @@
     </row>
     <row r="203" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A203" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B203" s="5">
         <v>0</v>
@@ -16770,7 +16770,7 @@
     </row>
     <row r="204" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A204" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B204" s="5">
         <v>0</v>
@@ -16847,7 +16847,7 @@
     </row>
     <row r="205" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A205" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B205" s="5">
         <v>0</v>
@@ -16924,13 +16924,13 @@
     </row>
     <row r="206" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A206" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B206" s="5">
+        <v>0</v>
+      </c>
+      <c r="C206" s="5" t="s">
         <v>179</v>
-      </c>
-      <c r="B206" s="5">
-        <v>0</v>
-      </c>
-      <c r="C206" s="5" t="s">
-        <v>180</v>
       </c>
       <c r="D206" s="1">
         <v>0</v>

</xml_diff>